<commit_message>
update another two table
</commit_message>
<xml_diff>
--- a/Data/branch_wise_aging_stock.xlsx
+++ b/Data/branch_wise_aging_stock.xlsx
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="AQ2" t="n">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="AR2" t="n">
         <v>243</v>
@@ -1058,7 +1058,7 @@
         <v>1697</v>
       </c>
       <c r="BH2" t="n">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="BI2" t="n">
         <v>120</v>
@@ -1588,7 +1588,7 @@
         <v>132</v>
       </c>
       <c r="AW4" t="n">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AX4" t="n">
         <v>169</v>
@@ -1908,7 +1908,7 @@
         <v>854</v>
       </c>
       <c r="BH5" t="n">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="BI5" t="n">
         <v>159</v>
@@ -2147,7 +2147,7 @@
         <v>338</v>
       </c>
       <c r="AR6" t="n">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="AS6" t="n">
         <v>734</v>
@@ -2195,7 +2195,7 @@
         <v>670</v>
       </c>
       <c r="BH6" t="n">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="BI6" t="n">
         <v>406</v>
@@ -2207,7 +2207,7 @@
         <v>552</v>
       </c>
       <c r="BL6" t="n">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="BM6" t="n">
         <v>801</v>
@@ -2216,7 +2216,7 @@
         <v>375</v>
       </c>
       <c r="BO6" t="n">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="BP6" t="n">
         <v>370</v>
@@ -2426,10 +2426,10 @@
         </is>
       </c>
       <c r="AQ7" t="n">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AR7" t="n">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="AS7" t="n">
         <v>794</v>
@@ -2447,7 +2447,7 @@
         <v>526</v>
       </c>
       <c r="AX7" t="n">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AY7" t="n">
         <v>312</v>
@@ -2462,7 +2462,7 @@
         <v>780</v>
       </c>
       <c r="BC7" t="n">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="BD7" t="n">
         <v>644</v>
@@ -2477,19 +2477,19 @@
         <v>463</v>
       </c>
       <c r="BH7" t="n">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="BI7" t="n">
         <v>613</v>
       </c>
       <c r="BJ7" t="n">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="BK7" t="n">
         <v>585</v>
       </c>
       <c r="BL7" t="n">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="BM7" t="n">
         <v>617</v>
@@ -2498,7 +2498,7 @@
         <v>290</v>
       </c>
       <c r="BO7" t="n">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="BP7" t="n">
         <v>382</v>
@@ -2510,7 +2510,7 @@
         <v>1083</v>
       </c>
       <c r="BT7" t="n">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="BU7" t="n">
         <v>418</v>
@@ -3045,7 +3045,7 @@
         <v>165</v>
       </c>
       <c r="BG9" t="n">
-        <v>1209</v>
+        <v>1077</v>
       </c>
       <c r="BH9" t="n">
         <v>228</v>
@@ -3060,16 +3060,16 @@
         <v>503</v>
       </c>
       <c r="BL9" t="n">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="BM9" t="n">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="BN9" t="n">
         <v>388</v>
       </c>
       <c r="BO9" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BP9" t="n">
         <v>350</v>
@@ -3574,7 +3574,7 @@
         <v>499</v>
       </c>
       <c r="AR11" t="n">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="AS11" t="n">
         <v>555</v>
@@ -3589,7 +3589,7 @@
         <v>143</v>
       </c>
       <c r="AW11" t="n">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AX11" t="n">
         <v>401</v>
@@ -3619,7 +3619,7 @@
         <v>445</v>
       </c>
       <c r="BG11" t="n">
-        <v>1886</v>
+        <v>1805</v>
       </c>
       <c r="BH11" t="n">
         <v>804</v>
@@ -3628,13 +3628,13 @@
         <v>416</v>
       </c>
       <c r="BJ11" t="n">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="BK11" t="n">
         <v>614</v>
       </c>
       <c r="BL11" t="n">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="BM11" t="n">
         <v>852</v>
@@ -3643,7 +3643,7 @@
         <v>678</v>
       </c>
       <c r="BO11" t="n">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="BP11" t="n">
         <v>471</v>
@@ -3937,7 +3937,7 @@
         <v>83</v>
       </c>
       <c r="BT12" t="n">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="BU12" t="n">
         <v>48</v>
@@ -4140,7 +4140,7 @@
         <v>1476</v>
       </c>
       <c r="AR13" t="n">
-        <v>1433</v>
+        <v>1427</v>
       </c>
       <c r="AS13" t="n">
         <v>1003</v>
@@ -4200,7 +4200,7 @@
         <v>1215</v>
       </c>
       <c r="BL13" t="n">
-        <v>428</v>
+        <v>398</v>
       </c>
       <c r="BM13" t="n">
         <v>979</v>
@@ -4209,7 +4209,7 @@
         <v>1319</v>
       </c>
       <c r="BO13" t="n">
-        <v>1656</v>
+        <v>1651</v>
       </c>
       <c r="BP13" t="n">
         <v>1920</v>
@@ -4224,7 +4224,7 @@
         <v>1441</v>
       </c>
       <c r="BT13" t="n">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="BU13" t="n">
         <v>1315</v>
@@ -4442,7 +4442,7 @@
         <v>2629</v>
       </c>
       <c r="AW14" t="n">
-        <v>2276</v>
+        <v>2270</v>
       </c>
       <c r="AX14" t="n">
         <v>2982</v>
@@ -4487,7 +4487,7 @@
         <v>1362</v>
       </c>
       <c r="BL14" t="n">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="BM14" t="n">
         <v>2475</v>
@@ -4496,7 +4496,7 @@
         <v>2305</v>
       </c>
       <c r="BO14" t="n">
-        <v>2057</v>
+        <v>2041</v>
       </c>
       <c r="BP14" t="n">
         <v>2518</v>
@@ -4511,7 +4511,7 @@
         <v>5450</v>
       </c>
       <c r="BT14" t="n">
-        <v>1485</v>
+        <v>1479</v>
       </c>
       <c r="BU14" t="n">
         <v>2779</v>
@@ -4714,7 +4714,7 @@
         <v>3265</v>
       </c>
       <c r="AR15" t="n">
-        <v>6441</v>
+        <v>6425</v>
       </c>
       <c r="AS15" t="n">
         <v>5997</v>
@@ -4729,10 +4729,10 @@
         <v>5362</v>
       </c>
       <c r="AW15" t="n">
-        <v>4107</v>
+        <v>4106</v>
       </c>
       <c r="AX15" t="n">
-        <v>6969</v>
+        <v>6962</v>
       </c>
       <c r="AY15" t="n">
         <v>6070</v>
@@ -4762,28 +4762,28 @@
         <v>4844</v>
       </c>
       <c r="BH15" t="n">
-        <v>4416</v>
+        <v>4414</v>
       </c>
       <c r="BI15" t="n">
         <v>3831</v>
       </c>
       <c r="BJ15" t="n">
-        <v>3799</v>
+        <v>3794</v>
       </c>
       <c r="BK15" t="n">
         <v>3355</v>
       </c>
       <c r="BL15" t="n">
-        <v>2556</v>
+        <v>2548</v>
       </c>
       <c r="BM15" t="n">
-        <v>3623</v>
+        <v>3619</v>
       </c>
       <c r="BN15" t="n">
         <v>5514</v>
       </c>
       <c r="BO15" t="n">
-        <v>2171</v>
+        <v>2169</v>
       </c>
       <c r="BP15" t="n">
         <v>3591</v>
@@ -4798,10 +4798,10 @@
         <v>199</v>
       </c>
       <c r="BT15" t="n">
-        <v>2075</v>
+        <v>2063</v>
       </c>
       <c r="BU15" t="n">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="BV15" t="n">
         <v>1752</v>
@@ -4998,10 +4998,10 @@
         </is>
       </c>
       <c r="AQ16" t="n">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="AR16" t="n">
-        <v>2289</v>
+        <v>2288</v>
       </c>
       <c r="AS16" t="n">
         <v>527</v>
@@ -5016,10 +5016,10 @@
         <v>1485</v>
       </c>
       <c r="AW16" t="n">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="AX16" t="n">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="AY16" t="n">
         <v>1820</v>
@@ -5049,28 +5049,28 @@
         <v>521</v>
       </c>
       <c r="BH16" t="n">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="BI16" t="n">
         <v>1204</v>
       </c>
       <c r="BJ16" t="n">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="BK16" t="n">
         <v>2140</v>
       </c>
       <c r="BL16" t="n">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="BM16" t="n">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="BN16" t="n">
         <v>1284</v>
       </c>
       <c r="BO16" t="n">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="BP16" t="n">
         <v>1523</v>
@@ -5288,7 +5288,7 @@
         <v>2688</v>
       </c>
       <c r="AR17" t="n">
-        <v>6749</v>
+        <v>6742</v>
       </c>
       <c r="AS17" t="n">
         <v>2706</v>
@@ -5303,10 +5303,10 @@
         <v>2166</v>
       </c>
       <c r="AW17" t="n">
-        <v>3055</v>
+        <v>3051</v>
       </c>
       <c r="AX17" t="n">
-        <v>3467</v>
+        <v>3464</v>
       </c>
       <c r="AY17" t="n">
         <v>5670</v>
@@ -5321,7 +5321,7 @@
         <v>2571</v>
       </c>
       <c r="BC17" t="n">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="BD17" t="n">
         <v>4557</v>
@@ -5336,28 +5336,28 @@
         <v>2605</v>
       </c>
       <c r="BH17" t="n">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="BI17" t="n">
         <v>3189</v>
       </c>
       <c r="BJ17" t="n">
-        <v>2960</v>
+        <v>2955</v>
       </c>
       <c r="BK17" t="n">
         <v>5951</v>
       </c>
       <c r="BL17" t="n">
-        <v>2555</v>
+        <v>2547</v>
       </c>
       <c r="BM17" t="n">
-        <v>2882</v>
+        <v>2877</v>
       </c>
       <c r="BN17" t="n">
         <v>4537</v>
       </c>
       <c r="BO17" t="n">
-        <v>2120</v>
+        <v>2117</v>
       </c>
       <c r="BP17" t="n">
         <v>2169</v>
@@ -5372,7 +5372,7 @@
         <v>17702</v>
       </c>
       <c r="BT17" t="n">
-        <v>1330</v>
+        <v>1322</v>
       </c>
       <c r="BU17" t="n">
         <v>3106</v>
@@ -6164,10 +6164,10 @@
         <v>9779</v>
       </c>
       <c r="AW20" t="n">
-        <v>7126</v>
+        <v>7124</v>
       </c>
       <c r="AX20" t="n">
-        <v>7951</v>
+        <v>7938</v>
       </c>
       <c r="AY20" t="n">
         <v>7714</v>
@@ -6194,10 +6194,10 @@
         <v>6944</v>
       </c>
       <c r="BG20" t="n">
-        <v>4963</v>
+        <v>3523</v>
       </c>
       <c r="BH20" t="n">
-        <v>3191</v>
+        <v>3189</v>
       </c>
       <c r="BI20" t="n">
         <v>5381</v>
@@ -6209,16 +6209,16 @@
         <v>7705</v>
       </c>
       <c r="BL20" t="n">
-        <v>8322</v>
+        <v>8318</v>
       </c>
       <c r="BM20" t="n">
-        <v>4311</v>
+        <v>4245</v>
       </c>
       <c r="BN20" t="n">
         <v>5411</v>
       </c>
       <c r="BO20" t="n">
-        <v>7042</v>
+        <v>7030</v>
       </c>
       <c r="BP20" t="n">
         <v>5707</v>
@@ -6233,7 +6233,7 @@
         <v>25095</v>
       </c>
       <c r="BT20" t="n">
-        <v>6535</v>
+        <v>6531</v>
       </c>
       <c r="BU20" t="n">
         <v>4394</v>
@@ -6436,7 +6436,7 @@
         <v>395</v>
       </c>
       <c r="AR21" t="n">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AS21" t="n">
         <v>74</v>
@@ -6451,10 +6451,10 @@
         <v>447</v>
       </c>
       <c r="AW21" t="n">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="AX21" t="n">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AY21" t="n">
         <v>346</v>
@@ -6469,7 +6469,7 @@
         <v>125</v>
       </c>
       <c r="BC21" t="n">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BD21" t="n">
         <v>114</v>
@@ -6496,7 +6496,7 @@
         <v>72</v>
       </c>
       <c r="BL21" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BM21" t="n">
         <v>106</v>
@@ -6723,7 +6723,7 @@
         <v>7144</v>
       </c>
       <c r="AR22" t="n">
-        <v>11339</v>
+        <v>11338</v>
       </c>
       <c r="AS22" t="n">
         <v>5631</v>
@@ -6738,10 +6738,10 @@
         <v>6673</v>
       </c>
       <c r="AW22" t="n">
-        <v>7077</v>
+        <v>7073</v>
       </c>
       <c r="AX22" t="n">
-        <v>5522</v>
+        <v>5518</v>
       </c>
       <c r="AY22" t="n">
         <v>9296</v>
@@ -6768,7 +6768,7 @@
         <v>5523</v>
       </c>
       <c r="BG22" t="n">
-        <v>5099</v>
+        <v>3299</v>
       </c>
       <c r="BH22" t="n">
         <v>3132</v>
@@ -6783,16 +6783,16 @@
         <v>4238</v>
       </c>
       <c r="BL22" t="n">
-        <v>7354</v>
+        <v>7345</v>
       </c>
       <c r="BM22" t="n">
-        <v>4124</v>
+        <v>4102</v>
       </c>
       <c r="BN22" t="n">
         <v>7411</v>
       </c>
       <c r="BO22" t="n">
-        <v>6599</v>
+        <v>6586</v>
       </c>
       <c r="BP22" t="n">
         <v>5126</v>
@@ -6807,10 +6807,10 @@
         <v>6348</v>
       </c>
       <c r="BT22" t="n">
-        <v>4286</v>
+        <v>4280</v>
       </c>
       <c r="BU22" t="n">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="BV22" t="n">
         <v>1037</v>
@@ -7043,7 +7043,7 @@
         <v>541</v>
       </c>
       <c r="BC23" t="n">
-        <v>952</v>
+        <v>902</v>
       </c>
       <c r="BD23" t="n">
         <v>310</v>
@@ -7330,7 +7330,7 @@
         <v>171</v>
       </c>
       <c r="BC24" t="n">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="BD24" t="n">
         <v>161</v>
@@ -7351,7 +7351,7 @@
         <v>213</v>
       </c>
       <c r="BJ24" t="n">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="BK24" t="n">
         <v>127</v>
@@ -7581,7 +7581,7 @@
         </is>
       </c>
       <c r="AQ25" t="n">
-        <v>5062</v>
+        <v>5052</v>
       </c>
       <c r="AR25" t="n">
         <v>4965</v>
@@ -7653,7 +7653,7 @@
         <v>4974</v>
       </c>
       <c r="BO25" t="n">
-        <v>3423</v>
+        <v>3418</v>
       </c>
       <c r="BP25" t="n">
         <v>3338</v>
@@ -7889,7 +7889,7 @@
         <v>1526</v>
       </c>
       <c r="AX26" t="n">
-        <v>1539</v>
+        <v>1499</v>
       </c>
       <c r="AY26" t="n">
         <v>9080</v>
@@ -9359,7 +9359,7 @@
         <v>57</v>
       </c>
       <c r="BO31" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BP31" t="n">
         <v>95</v>
@@ -9653,7 +9653,7 @@
         <v>58</v>
       </c>
       <c r="BT32" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="BU32" t="n">
         <v>42</v>
@@ -10130,7 +10130,7 @@
         <v>326</v>
       </c>
       <c r="AR34" t="n">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AS34" t="n">
         <v>63</v>
@@ -10163,7 +10163,7 @@
         <v>345</v>
       </c>
       <c r="BC34" t="n">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="BD34" t="n">
         <v>182</v>
@@ -10196,7 +10196,7 @@
         <v>329</v>
       </c>
       <c r="BO34" t="n">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="BP34" t="n">
         <v>162</v>
@@ -10211,7 +10211,7 @@
         <v>13566</v>
       </c>
       <c r="BT34" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BU34" t="n">
         <v>220</v>
@@ -10490,7 +10490,7 @@
         <v>61</v>
       </c>
       <c r="BT35" t="n">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BU35" t="n">
         <v>110</v>
@@ -11020,7 +11020,7 @@
         <v>241</v>
       </c>
       <c r="BH37" t="n">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="BI37" t="n">
         <v>155</v>
@@ -11292,7 +11292,7 @@
         <v>842</v>
       </c>
       <c r="BC38" t="n">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="BD38" t="n">
         <v>339</v>
@@ -11307,7 +11307,7 @@
         <v>25</v>
       </c>
       <c r="BH38" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="BI38" t="n">
         <v>637</v>
@@ -11328,7 +11328,7 @@
         <v>535</v>
       </c>
       <c r="BO38" t="n">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="BP38" t="n">
         <v>1249</v>
@@ -11343,10 +11343,10 @@
         <v>1738</v>
       </c>
       <c r="BT38" t="n">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="BU38" t="n">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="BV38" t="n">
         <v>847</v>
@@ -11630,7 +11630,7 @@
         <v>3188</v>
       </c>
       <c r="BT39" t="n">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="BU39" t="n">
         <v>1082</v>
@@ -11833,7 +11833,7 @@
         <v>513</v>
       </c>
       <c r="AR40" t="n">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="AS40" t="n">
         <v>1091</v>
@@ -11866,7 +11866,7 @@
         <v>669</v>
       </c>
       <c r="BC40" t="n">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="BD40" t="n">
         <v>506</v>
@@ -11878,10 +11878,10 @@
         <v>202</v>
       </c>
       <c r="BG40" t="n">
-        <v>8357</v>
+        <v>8069</v>
       </c>
       <c r="BH40" t="n">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="BI40" t="n">
         <v>639</v>
@@ -11902,7 +11902,7 @@
         <v>758</v>
       </c>
       <c r="BO40" t="n">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="BP40" t="n">
         <v>465</v>
@@ -11917,7 +11917,7 @@
         <v>4703</v>
       </c>
       <c r="BT40" t="n">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="BU40" t="n">
         <v>994</v>
@@ -12168,7 +12168,7 @@
         <v>3753</v>
       </c>
       <c r="BH41" t="n">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="BI41" t="n">
         <v>1223</v>
@@ -12180,7 +12180,7 @@
         <v>2137</v>
       </c>
       <c r="BL41" t="n">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="BM41" t="n">
         <v>1020</v>
@@ -12189,7 +12189,7 @@
         <v>975</v>
       </c>
       <c r="BO41" t="n">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="BP41" t="n">
         <v>1542</v>
@@ -12204,7 +12204,7 @@
         <v>14865</v>
       </c>
       <c r="BT41" t="n">
-        <v>1520</v>
+        <v>1517</v>
       </c>
       <c r="BU41" t="n">
         <v>1161</v>
@@ -12491,7 +12491,7 @@
         <v>110</v>
       </c>
       <c r="BT42" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BU42" t="n">
         <v>64</v>
@@ -12946,7 +12946,7 @@
         <v>365</v>
       </c>
       <c r="AX44" t="n">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="AY44" t="n">
         <v>192</v>
@@ -12961,7 +12961,7 @@
         <v>412</v>
       </c>
       <c r="BC44" t="n">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="BD44" t="n">
         <v>541</v>
@@ -12976,7 +12976,7 @@
         <v>523</v>
       </c>
       <c r="BH44" t="n">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="BI44" t="n">
         <v>686</v>
@@ -12988,16 +12988,16 @@
         <v>498</v>
       </c>
       <c r="BL44" t="n">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="BM44" t="n">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="BN44" t="n">
         <v>793</v>
       </c>
       <c r="BO44" t="n">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="BP44" t="n">
         <v>639</v>
@@ -13230,7 +13230,7 @@
         <v>1952</v>
       </c>
       <c r="AX45" t="n">
-        <v>2790</v>
+        <v>2787</v>
       </c>
       <c r="AY45" t="n">
         <v>2750</v>
@@ -13272,7 +13272,7 @@
         <v>1483</v>
       </c>
       <c r="BL45" t="n">
-        <v>1601</v>
+        <v>1594</v>
       </c>
       <c r="BM45" t="n">
         <v>2256</v>
@@ -14127,16 +14127,16 @@
         <v>350</v>
       </c>
       <c r="BJ48" t="n">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="BK48" t="n">
         <v>336</v>
       </c>
       <c r="BL48" t="n">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BM48" t="n">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="BN48" t="n">
         <v>614</v>
@@ -14157,7 +14157,7 @@
         <v>15</v>
       </c>
       <c r="BT48" t="n">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="BU48" t="n">
         <v>231</v>
@@ -14405,7 +14405,7 @@
         <v>53</v>
       </c>
       <c r="BG49" t="n">
-        <v>3231</v>
+        <v>3111</v>
       </c>
       <c r="BH49" t="n">
         <v>36</v>
@@ -14707,10 +14707,10 @@
         <v>1002</v>
       </c>
       <c r="BL50" t="n">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="BM50" t="n">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="BN50" t="n">
         <v>1256</v>
@@ -14731,7 +14731,7 @@
         <v>400</v>
       </c>
       <c r="BT50" t="n">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="BU50" t="n">
         <v>1236</v>
@@ -15536,7 +15536,7 @@
         <v>2417</v>
       </c>
       <c r="BT53" t="n">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="BU53" t="n">
         <v>719</v>
@@ -16185,13 +16185,13 @@
         <v>934</v>
       </c>
       <c r="BH56" t="n">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="BI56" t="n">
         <v>3844</v>
       </c>
       <c r="BJ56" t="n">
-        <v>2502</v>
+        <v>2493</v>
       </c>
       <c r="BK56" t="n">
         <v>2154</v>
@@ -17276,7 +17276,7 @@
         <v>115</v>
       </c>
       <c r="AW60" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AX60" t="n">
         <v>118</v>
@@ -17294,7 +17294,7 @@
         <v>131</v>
       </c>
       <c r="BC60" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="BD60" t="n">
         <v>274</v>
@@ -17666,7 +17666,7 @@
         <v>1273</v>
       </c>
       <c r="BL62" t="n">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="BM62" t="n">
         <v>1517</v>
@@ -17675,7 +17675,7 @@
         <v>1476</v>
       </c>
       <c r="BO62" t="n">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="BP62" t="n">
         <v>1189</v>
@@ -17687,7 +17687,7 @@
         <v>2151</v>
       </c>
       <c r="BT62" t="n">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="BU62" t="n">
         <v>572</v>
@@ -18229,7 +18229,7 @@
         <v>290</v>
       </c>
       <c r="BL64" t="n">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="BM64" t="n">
         <v>695</v>
@@ -18238,7 +18238,7 @@
         <v>400</v>
       </c>
       <c r="BO64" t="n">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="BP64" t="n">
         <v>745</v>
@@ -18253,7 +18253,7 @@
         <v>9</v>
       </c>
       <c r="BT64" t="n">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="BU64" t="n">
         <v>516</v>
@@ -19041,13 +19041,13 @@
         <v>3976</v>
       </c>
       <c r="BH67" t="n">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="BI67" t="n">
         <v>321</v>
       </c>
       <c r="BJ67" t="n">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="BK67" t="n">
         <v>1306</v>
@@ -19287,10 +19287,10 @@
         <v>380</v>
       </c>
       <c r="AW68" t="n">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AX68" t="n">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AY68" t="n">
         <v>307</v>
@@ -19353,7 +19353,7 @@
         <v>430</v>
       </c>
       <c r="BT68" t="n">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BU68" t="n">
         <v>283</v>
@@ -19632,7 +19632,7 @@
         <v>365</v>
       </c>
       <c r="BT69" t="n">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="BU69" t="n">
         <v>640</v>
@@ -19887,7 +19887,7 @@
         <v>55</v>
       </c>
       <c r="BL70" t="n">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BM70" t="n">
         <v>32</v>
@@ -20183,7 +20183,7 @@
         <v>596</v>
       </c>
       <c r="BO71" t="n">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="BP71" t="n">
         <v>1087</v>
@@ -20723,7 +20723,7 @@
         <v>1359</v>
       </c>
       <c r="BO73" t="n">
-        <v>954</v>
+        <v>932</v>
       </c>
       <c r="BP73" t="n">
         <v>2965</v>
@@ -20962,7 +20962,7 @@
         <v>107</v>
       </c>
       <c r="BO74" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BP74" t="n">
         <v>128</v>
@@ -21243,7 +21243,7 @@
         <v>391</v>
       </c>
       <c r="BO75" t="n">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="BP75" t="n">
         <v>291</v>
@@ -21681,7 +21681,7 @@
         </is>
       </c>
       <c r="AQ77" t="n">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AR77" t="n">
         <v>207</v>
@@ -21753,7 +21753,7 @@
         <v>82</v>
       </c>
       <c r="BO77" t="n">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="BP77" t="n">
         <v>342</v>
@@ -22031,7 +22031,7 @@
         <v>1861</v>
       </c>
       <c r="BL78" t="n">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="BM78" t="n">
         <v>1321</v>
@@ -22318,7 +22318,7 @@
         <v>700</v>
       </c>
       <c r="BL79" t="n">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="BM79" t="n">
         <v>1070</v>
@@ -22342,7 +22342,7 @@
         <v>33</v>
       </c>
       <c r="BT79" t="n">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="BU79" t="n">
         <v>1431</v>
@@ -22558,7 +22558,7 @@
         <v>2180</v>
       </c>
       <c r="AX80" t="n">
-        <v>2427</v>
+        <v>2406</v>
       </c>
       <c r="AY80" t="n">
         <v>2837</v>
@@ -22588,7 +22588,7 @@
         <v>2695</v>
       </c>
       <c r="BH80" t="n">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="BI80" t="n">
         <v>1176</v>
@@ -22600,7 +22600,7 @@
         <v>1464</v>
       </c>
       <c r="BL80" t="n">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="BM80" t="n">
         <v>2340</v>
@@ -22824,7 +22824,7 @@
         <v>4463</v>
       </c>
       <c r="AR81" t="n">
-        <v>8196</v>
+        <v>8194</v>
       </c>
       <c r="AS81" t="n">
         <v>4277</v>
@@ -22842,7 +22842,7 @@
         <v>5405</v>
       </c>
       <c r="AX81" t="n">
-        <v>4033</v>
+        <v>4032</v>
       </c>
       <c r="AY81" t="n">
         <v>5103</v>
@@ -22878,13 +22878,13 @@
         <v>4698</v>
       </c>
       <c r="BJ81" t="n">
-        <v>3697</v>
+        <v>3696</v>
       </c>
       <c r="BK81" t="n">
         <v>3651</v>
       </c>
       <c r="BL81" t="n">
-        <v>3268</v>
+        <v>3267</v>
       </c>
       <c r="BM81" t="n">
         <v>4873</v>
@@ -22908,10 +22908,10 @@
         <v>1024</v>
       </c>
       <c r="BT81" t="n">
-        <v>5015</v>
+        <v>5009</v>
       </c>
       <c r="BU81" t="n">
-        <v>2267</v>
+        <v>2266</v>
       </c>
       <c r="BV81" t="n">
         <v>2904</v>

</xml_diff>